<commit_message>
ENH: add a checkbox to choose if the user wants the complementary angle.
</commit_message>
<xml_diff>
--- a/AQ3DC/Resources/name_landmark.xlsx
+++ b/AQ3DC/Resources/name_landmark.xlsx
@@ -650,11 +650,12 @@
   <dimension ref="A1:AJ53"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
+      <selection pane="topLeft" activeCell="C24" activeCellId="0" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.66796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.67578125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.33"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
STYLE : change 2 names of landmark
</commit_message>
<xml_diff>
--- a/AQ3DC/Resources/name_landmark.xlsx
+++ b/AQ3DC/Resources/name_landmark.xlsx
@@ -650,10 +650,10 @@
   <dimension ref="A1:AJ53"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C24" activeCellId="0" sqref="C24"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.67578125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.33"/>

</xml_diff>

<commit_message>
PERF : new wy to calculate roll and yaw angle + change name landmark
</commit_message>
<xml_diff>
--- a/AQ3DC/Resources/name_landmark.xlsx
+++ b/AQ3DC/Resources/name_landmark.xlsx
@@ -112,7 +112,7 @@
     <t xml:space="preserve">UR4</t>
   </si>
   <si>
-    <t xml:space="preserve">Rco</t>
+    <t xml:space="preserve">RCo</t>
   </si>
   <si>
     <t xml:space="preserve">RMZyg</t>
@@ -130,7 +130,7 @@
     <t xml:space="preserve">UR3</t>
   </si>
   <si>
-    <t xml:space="preserve">Lco</t>
+    <t xml:space="preserve">LCo</t>
   </si>
   <si>
     <t xml:space="preserve">LMZyg</t>
@@ -650,10 +650,10 @@
   <dimension ref="A1:AJ53"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.33"/>

</xml_diff>

<commit_message>
BUG : name Pog delete space
</commit_message>
<xml_diff>
--- a/AQ3DC/Resources/name_landmark.xlsx
+++ b/AQ3DC/Resources/name_landmark.xlsx
@@ -301,7 +301,7 @@
     <t xml:space="preserve">B</t>
   </si>
   <si>
-    <t xml:space="preserve">Pog </t>
+    <t xml:space="preserve">Pog</t>
   </si>
   <si>
     <t xml:space="preserve">Gn</t>
@@ -650,10 +650,10 @@
   <dimension ref="A1:AJ53"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="topLeft" activeCell="A24" activeCellId="0" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.33"/>

</xml_diff>